<commit_message>
Dashboard Report and Pivot tables
</commit_message>
<xml_diff>
--- a/Dashboard.xlsx
+++ b/Dashboard.xlsx
@@ -1244,6 +1244,9 @@
             </a:outerShdw>
           </a:effectLst>
         </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:layout/>
@@ -1541,12 +1544,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="133614208"/>
-        <c:axId val="161317248"/>
+        <c:axId val="127186432"/>
+        <c:axId val="127187968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133614208"/>
+        <c:axId val="127186432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1574,14 +1576,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161317248"/>
+        <c:crossAx val="127187968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="161317248"/>
+        <c:axId val="127187968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1621,7 +1623,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133614208"/>
+        <c:crossAx val="127186432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1642,7 +1644,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1730,25 +1732,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="126187776"/>
-        <c:axId val="126189568"/>
+        <c:axId val="128026112"/>
+        <c:axId val="128027648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="126187776"/>
+        <c:axId val="128026112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126189568"/>
+        <c:crossAx val="128027648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126189568"/>
+        <c:axId val="128027648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1756,7 +1758,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126187776"/>
+        <c:crossAx val="128026112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1765,7 +1767,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1859,7 +1861,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1883,7 +1885,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:dLblPos val="inEnd"/>
           <c:showVal val="1"/>
         </c:dLbl>
@@ -1975,25 +1976,25 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="75"/>
-        <c:axId val="126268544"/>
-        <c:axId val="126270080"/>
+        <c:axId val="128078592"/>
+        <c:axId val="128080128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="126268544"/>
+        <c:axId val="128078592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126270080"/>
+        <c:crossAx val="128080128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126270080"/>
+        <c:axId val="128080128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2002,7 +2003,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126268544"/>
+        <c:crossAx val="128078592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2011,7 +2012,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2107,28 +2108,27 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:dropLines/>
         <c:marker val="1"/>
-        <c:axId val="126288640"/>
-        <c:axId val="126290176"/>
+        <c:axId val="128127744"/>
+        <c:axId val="128129280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126288640"/>
+        <c:axId val="128127744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126290176"/>
+        <c:crossAx val="128129280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126290176"/>
+        <c:axId val="128129280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2136,7 +2136,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126288640"/>
+        <c:crossAx val="128127744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2145,7 +2145,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2217,24 +2217,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="126313600"/>
-        <c:axId val="126315136"/>
+        <c:axId val="128140416"/>
+        <c:axId val="128141952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="126313600"/>
+        <c:axId val="128140416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126315136"/>
+        <c:crossAx val="128141952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126315136"/>
+        <c:axId val="128141952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2242,7 +2242,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126313600"/>
+        <c:crossAx val="128140416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2251,7 +2251,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2319,7 +2319,7 @@
           <c:layout>
             <c:manualLayout>
               <c:x val="0.10921501706484642"/>
-              <c:y val="1.5209125475285183E-2"/>
+              <c:y val="1.5209125475285185E-2"/>
             </c:manualLayout>
           </c:layout>
           <c:tx>
@@ -2464,7 +2464,7 @@
           <c:layout>
             <c:manualLayout>
               <c:x val="0.10921501706484642"/>
-              <c:y val="1.5209125475285183E-2"/>
+              <c:y val="1.5209125475285185E-2"/>
             </c:manualLayout>
           </c:layout>
           <c:tx>
@@ -2573,7 +2573,7 @@
           <c:layout>
             <c:manualLayout>
               <c:x val="0.10921501706484642"/>
-              <c:y val="1.5209125475285183E-2"/>
+              <c:y val="1.5209125475285185E-2"/>
             </c:manualLayout>
           </c:layout>
           <c:tx>
@@ -2602,10 +2602,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14154330708661417"/>
-          <c:y val="3.8297031052936567E-2"/>
-          <c:w val="0.76673506720750872"/>
-          <c:h val="0.90725225083916272"/>
+          <c:x val="0.14154330708661422"/>
+          <c:y val="3.8297031052936574E-2"/>
+          <c:w val="0.76673506720750884"/>
+          <c:h val="0.90725225083916261"/>
         </c:manualLayout>
       </c:layout>
       <c:doughnutChart>
@@ -2689,7 +2689,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="0.10921501706484642"/>
-                  <c:y val="1.5209125475285183E-2"/>
+                  <c:y val="1.5209125475285185E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -2774,8 +2774,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.42565360604824798"/>
           <c:y val="0.360175641551915"/>
-          <c:w val="0.18282690759272618"/>
-          <c:h val="0.26376136632210073"/>
+          <c:w val="0.18282690759272624"/>
+          <c:h val="0.26376136632210079"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -2789,7 +2789,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2973,7 +2973,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.2717910328091047E-2"/>
+          <c:x val="5.2717910328091075E-2"/>
           <c:y val="5.0538465300533082E-2"/>
           <c:w val="0.92711825454222141"/>
           <c:h val="0.80106812735364596"/>
@@ -3079,11 +3079,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="75"/>
-        <c:axId val="73605120"/>
-        <c:axId val="74617600"/>
+        <c:axId val="127541632"/>
+        <c:axId val="127543168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="73605120"/>
+        <c:axId val="127541632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3111,14 +3111,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74617600"/>
+        <c:crossAx val="127543168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74617600"/>
+        <c:axId val="127543168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3158,7 +3158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73605120"/>
+        <c:crossAx val="127541632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3178,7 +3178,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3385,10 +3385,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.23725309336332959"/>
+          <c:x val="0.23725309336332961"/>
           <c:y val="0"/>
-          <c:w val="0.71004461942257213"/>
-          <c:h val="0.88325097903656014"/>
+          <c:w val="0.71004461942257235"/>
+          <c:h val="0.88325097903656002"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3476,11 +3476,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="72836992"/>
-        <c:axId val="71893760"/>
+        <c:axId val="127582208"/>
+        <c:axId val="127568128"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="71893760"/>
+        <c:axId val="127568128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3498,11 +3498,12 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72836992"/>
+        <c:crossAx val="127582208"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="72836992"/>
+        <c:axId val="127582208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3529,7 +3530,8 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71893760"/>
+        <c:crossAx val="127568128"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3551,7 +3553,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3835,8 +3837,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13124249085902384"/>
-          <c:y val="4.7306270435496747E-2"/>
+          <c:x val="0.1312424908590239"/>
+          <c:y val="4.7306270435496775E-2"/>
           <c:w val="0.85006575790929362"/>
           <c:h val="0.79725434734441025"/>
         </c:manualLayout>
@@ -3959,11 +3961,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="98569216"/>
-        <c:axId val="133586944"/>
+        <c:axId val="127638528"/>
+        <c:axId val="127652608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98569216"/>
+        <c:axId val="127638528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3991,14 +3993,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133586944"/>
+        <c:crossAx val="127652608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133586944"/>
+        <c:axId val="127652608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4038,7 +4040,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98569216"/>
+        <c:crossAx val="127638528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4058,7 +4060,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4128,7 +4130,7 @@
           <c:layout>
             <c:manualLayout>
               <c:x val="0.23324073490813649"/>
-              <c:y val="-0.25798889892861804"/>
+              <c:y val="-0.25798889892861815"/>
             </c:manualLayout>
           </c:layout>
           <c:spPr/>
@@ -4426,7 +4428,7 @@
           <c:layout>
             <c:manualLayout>
               <c:x val="0.23324073490813649"/>
-              <c:y val="-0.25798889892861804"/>
+              <c:y val="-0.25798889892861815"/>
             </c:manualLayout>
           </c:layout>
           <c:spPr/>
@@ -4615,7 +4617,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr/>
           <c:txPr>
             <a:bodyPr/>
@@ -4657,7 +4658,7 @@
           <c:layout>
             <c:manualLayout>
               <c:x val="-0.14719293562880911"/>
-              <c:y val="0.12732467362865782"/>
+              <c:y val="0.12732467362865776"/>
             </c:manualLayout>
           </c:layout>
           <c:dLblPos val="bestFit"/>
@@ -4686,8 +4687,8 @@
           <c:idx val="0"/>
           <c:layout>
             <c:manualLayout>
-              <c:x val="-0.15910182837314826"/>
-              <c:y val="9.1435829053307049E-2"/>
+              <c:x val="-0.15910182837314824"/>
+              <c:y val="9.1435829053307063E-2"/>
             </c:manualLayout>
           </c:layout>
           <c:dLblPos val="bestFit"/>
@@ -4716,7 +4717,7 @@
           <c:idx val="0"/>
           <c:layout>
             <c:manualLayout>
-              <c:x val="-0.15654655456203567"/>
+              <c:x val="-0.15654655456203576"/>
               <c:y val="-4.900195313875351E-2"/>
             </c:manualLayout>
           </c:layout>
@@ -4732,7 +4733,7 @@
           <c:layout>
             <c:manualLayout>
               <c:x val="0.20464776902887138"/>
-              <c:y val="-0.21741638099845112"/>
+              <c:y val="-0.2174163809984512"/>
             </c:manualLayout>
           </c:layout>
           <c:dLblPos val="bestFit"/>
@@ -4747,10 +4748,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17551614743809199"/>
+          <c:x val="0.17551614743809202"/>
           <c:y val="0"/>
-          <c:w val="0.67584480200844455"/>
-          <c:h val="0.98382405805903317"/>
+          <c:w val="0.67584480200844488"/>
+          <c:h val="0.98382405805903328"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -4840,7 +4841,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-0.14719293562880911"/>
-                  <c:y val="0.12732467362865782"/>
+                  <c:y val="0.12732467362865776"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -4851,8 +4852,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.15910182837314826"/>
-                  <c:y val="9.1435829053307049E-2"/>
+                  <c:x val="-0.15910182837314824"/>
+                  <c:y val="9.1435829053307063E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -4863,7 +4864,7 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.15654655456203567"/>
+                  <c:x val="-0.15654655456203576"/>
                   <c:y val="-4.900195313875351E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -4876,7 +4877,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="0.20464776902887138"/>
-                  <c:y val="-0.21741638099845112"/>
+                  <c:y val="-0.2174163809984512"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -4958,7 +4959,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5018,9 +5019,6 @@
       <c:pivotFmt>
         <c:idx val="7"/>
         <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="002060"/>
-          </a:solidFill>
           <a:effectLst>
             <a:outerShdw blurRad="50800" dist="101600" dir="2700000" algn="tl" rotWithShape="0">
               <a:prstClr val="black">
@@ -5057,9 +5055,6 @@
       <c:pivotFmt>
         <c:idx val="8"/>
         <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="002060"/>
-          </a:solidFill>
           <a:ln w="38100">
             <a:solidFill>
               <a:srgbClr val="002060"/>
@@ -5073,22 +5068,10 @@
             </a:outerShdw>
           </a:effectLst>
         </c:spPr>
-        <c:marker>
-          <c:spPr>
-            <a:ln w="38100">
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="9"/>
         <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="002060"/>
-          </a:solidFill>
           <a:ln w="38100">
             <a:solidFill>
               <a:srgbClr val="002060"/>
@@ -5102,22 +5085,10 @@
             </a:outerShdw>
           </a:effectLst>
         </c:spPr>
-        <c:marker>
-          <c:spPr>
-            <a:ln w="38100">
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="10"/>
         <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="002060"/>
-          </a:solidFill>
           <a:ln w="38100">
             <a:solidFill>
               <a:srgbClr val="002060"/>
@@ -5131,22 +5102,10 @@
             </a:outerShdw>
           </a:effectLst>
         </c:spPr>
-        <c:marker>
-          <c:spPr>
-            <a:ln w="38100">
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="11"/>
         <c:spPr>
-          <a:solidFill>
-            <a:srgbClr val="002060"/>
-          </a:solidFill>
           <a:ln w="38100">
             <a:solidFill>
               <a:srgbClr val="002060"/>
@@ -5160,15 +5119,6 @@
             </a:outerShdw>
           </a:effectLst>
         </c:spPr>
-        <c:marker>
-          <c:spPr>
-            <a:ln w="38100">
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:marker>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -5178,9 +5128,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="6.3962788403955889E-2"/>
-          <c:y val="3.507195221286994E-2"/>
-          <c:w val="0.93213319177759923"/>
-          <c:h val="0.77954520771110503"/>
+          <c:y val="3.5071952212869954E-2"/>
+          <c:w val="0.93213319177759912"/>
+          <c:h val="0.77954520771110514"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -5200,9 +5150,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="002060"/>
-            </a:solidFill>
             <a:effectLst>
               <a:outerShdw blurRad="50800" dist="101600" dir="2700000" algn="tl" rotWithShape="0">
                 <a:prstClr val="black">
@@ -5216,11 +5163,7 @@
           </c:marker>
           <c:dPt>
             <c:idx val="1"/>
-            <c:marker/>
             <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
               <a:ln w="38100">
                 <a:solidFill>
                   <a:srgbClr val="002060"/>
@@ -5237,11 +5180,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:marker/>
             <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
               <a:ln w="38100">
                 <a:solidFill>
                   <a:srgbClr val="002060"/>
@@ -5258,11 +5197,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
-            <c:marker/>
             <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
               <a:ln w="38100">
                 <a:solidFill>
                   <a:srgbClr val="002060"/>
@@ -5279,11 +5214,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
-            <c:marker/>
             <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
               <a:ln w="38100">
                 <a:solidFill>
                   <a:srgbClr val="002060"/>
@@ -5365,7 +5296,6 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:dropLines>
           <c:spPr>
             <a:ln>
@@ -5379,11 +5309,11 @@
           </c:spPr>
         </c:dropLines>
         <c:marker val="1"/>
-        <c:axId val="124921344"/>
-        <c:axId val="124922880"/>
+        <c:axId val="127738240"/>
+        <c:axId val="127739776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="124921344"/>
+        <c:axId val="127738240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5411,14 +5341,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124922880"/>
+        <c:crossAx val="127739776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124922880"/>
+        <c:axId val="127739776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5457,7 +5387,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="124921344"/>
+        <c:crossAx val="127738240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5474,7 +5404,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5498,7 +5428,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr/>
           <c:txPr>
             <a:bodyPr/>
@@ -5586,13 +5515,12 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5674,25 +5602,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="126166144"/>
-        <c:axId val="126167680"/>
+        <c:axId val="128001152"/>
+        <c:axId val="128002688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="126166144"/>
+        <c:axId val="128001152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126167680"/>
+        <c:crossAx val="128002688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126167680"/>
+        <c:axId val="128002688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5701,7 +5629,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126166144"/>
+        <c:crossAx val="128001152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5710,7 +5638,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6081,7 +6009,7 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> STUDY ON CUSTOMER'S PREFERENCE AND AWARENESS TOWARDS THE RECENT MODE OF PAYMENT IN ONLINE SHOPPING</a:t>
+            <a:t> STUDY ON CUSTOMER'S PREFERENCE AND AWARENESS TOWARDS THE RECENT MODES OF PAYMENT IN ONLINE SHOPPING</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1800" b="1">
             <a:solidFill>
@@ -8916,438 +8844,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="9">
-  <location ref="B21:C26" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="24">
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="6">
-        <item x="1"/>
-        <item m="1" x="3"/>
-        <item x="0"/>
-        <item m="1" x="4"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="5"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of RESPONDENTS" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="5">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="8" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="8" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="8" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="5">
-  <location ref="B13:C17" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="24">
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="11"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of RESPONDENTS" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="7">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="11" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="11" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="11" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="11" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="9">
-  <location ref="H27:I34" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="24">
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="6">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="14"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of RESPONDENTS" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="8">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="8" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="8" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="8" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="8" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="8" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="9">
   <location ref="H4:I10" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="24">
@@ -9499,7 +8995,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="H14:I21" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="24">
@@ -9607,7 +9103,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="B30:C36" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="24">
@@ -9759,7 +9255,274 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="9">
+  <location ref="B21:C26" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="24">
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="6">
+        <item x="1"/>
+        <item m="1" x="3"/>
+        <item x="0"/>
+        <item m="1" x="4"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of RESPONDENTS" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="8" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="8" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="8" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="5">
+  <location ref="B13:C17" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="24">
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="11"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of RESPONDENTS" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="7">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="11" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="11" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="11" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="11" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="9">
   <location ref="B5:C9" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="24">
@@ -9853,6 +9616,171 @@
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="9">
+  <location ref="H27:I34" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="24">
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="6">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="14"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of RESPONDENTS" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="8">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="8" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="8" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="8" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="8" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="8" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="4"/>
           </reference>
         </references>
       </pivotArea>

</xml_diff>